<commit_message>
Made changes for mobile execution engine for youtube demo purpose
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine_Mobile.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine_Mobile.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="63">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -85,9 +85,6 @@
     <t>minput</t>
   </si>
   <si>
-    <t>btn_Createaccount</t>
-  </si>
-  <si>
     <t>Click button btn_Createaccount</t>
   </si>
   <si>
@@ -97,15 +94,9 @@
     <t>Enter First Name in First Name field</t>
   </si>
   <si>
-    <t>txt_Firstname</t>
-  </si>
-  <si>
     <t>Verify the webelement txt_Firstname</t>
   </si>
   <si>
-    <t>txt_Lastname</t>
-  </si>
-  <si>
     <t>Verify the webelement txt_Lastname</t>
   </si>
   <si>
@@ -133,9 +124,6 @@
     <t>Web Testing Facebook Account</t>
   </si>
   <si>
-    <t>Mobile Testing Facebook Account</t>
-  </si>
-  <si>
     <t>Web_Facebook</t>
   </si>
   <si>
@@ -190,24 +178,44 @@
     <t>mcloseBrowser</t>
   </si>
   <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>waitFor</t>
+  </si>
+  <si>
+    <t>TS_010</t>
+  </si>
+  <si>
+    <t>TS_011</t>
+  </si>
+  <si>
+    <t>txt_Email</t>
+  </si>
+  <si>
+    <t>txt_Password</t>
+  </si>
+  <si>
+    <t>btn_Login</t>
+  </si>
+  <si>
+    <t>Click on login button</t>
+  </si>
+  <si>
+    <t>Chakradhar23342</t>
+  </si>
+  <si>
+    <t>Mobile Web Testing Facebook Account</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>Wait</t>
-  </si>
-  <si>
-    <t>waitFor</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,15 +270,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -293,32 +307,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -615,461 +671,515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="21.1796875" collapsed="true"/>
-    <col min="2" max="2" style="7" width="8.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="7" width="51.90625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="7" width="18.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="7" width="22.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="7" width="24.90625" collapsed="true"/>
-    <col min="7" max="16384" style="7" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="21.1796875" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.7265625" style="8" collapsed="1"/>
+    <col min="3" max="3" width="51.90625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.453125" style="8" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.90625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.7265625" style="8" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="C4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="11"/>
+      <c r="G6" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7" t="s">
+      <c r="D15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="E18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7" t="s">
+      <c r="B19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="E19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="F20" s="12"/>
+      <c r="G20" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="F21" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="G21" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="C24" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="9" t="s">
+      <c r="D24" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="E24" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="7" t="s">
-        <v>56</v>
+      <c r="F24" s="11"/>
+      <c r="G24" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FAIL">
+  <conditionalFormatting sqref="G1 G24:G1048576 G3:G11 G15:G22 G13">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G23">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",G23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",G12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,10 +1197,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="21.1796875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="41.1796875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="12.6328125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="21.1796875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.1796875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.6328125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.7265625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1109,30 +1219,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added method for App opening in mobile and added new test data sheet for app methods
</commit_message>
<xml_diff>
--- a/KeywordDriven/src/test/java/dataEngine/DataEngine_Mobile.xlsx
+++ b/KeywordDriven/src/test/java/dataEngine/DataEngine_Mobile.xlsx
@@ -76,139 +76,139 @@
     <t>Open Browser</t>
   </si>
   <si>
+    <t>mverifyElement</t>
+  </si>
+  <si>
+    <t>minput</t>
+  </si>
+  <si>
+    <t>Click button btn_Createaccount</t>
+  </si>
+  <si>
+    <t>mclick</t>
+  </si>
+  <si>
+    <t>Enter First Name in First Name field</t>
+  </si>
+  <si>
+    <t>Verify the webelement txt_Firstname</t>
+  </si>
+  <si>
+    <t>Verify the webelement txt_Lastname</t>
+  </si>
+  <si>
+    <t>Enter Last Name in txt_Lastname field</t>
+  </si>
+  <si>
+    <t>Ravikanth</t>
+  </si>
+  <si>
+    <t>Edamakanti</t>
+  </si>
+  <si>
+    <t>Click on Next button</t>
+  </si>
+  <si>
+    <t>Navigate to Facebook</t>
+  </si>
+  <si>
+    <t>mnavigate</t>
+  </si>
+  <si>
+    <t>Mobile_Facebook</t>
+  </si>
+  <si>
+    <t>Web Testing Facebook Account</t>
+  </si>
+  <si>
+    <t>Web_Facebook</t>
+  </si>
+  <si>
+    <t>Testing Facebook using Real Mobile Phone</t>
+  </si>
+  <si>
+    <t>Testing Facebook using Web Browser</t>
+  </si>
+  <si>
+    <t>TS_002</t>
+  </si>
+  <si>
+    <t>openBrowser</t>
+  </si>
+  <si>
+    <t>navigate</t>
+  </si>
+  <si>
+    <t>m_btn_Createaccount</t>
+  </si>
+  <si>
+    <t>m_txt_Firstname</t>
+  </si>
+  <si>
+    <t>m_txt_Lastname</t>
+  </si>
+  <si>
+    <t>m_btn_Next</t>
+  </si>
+  <si>
+    <t>verifyElement</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>click</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>Close Broswer</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>TS_009</t>
+  </si>
+  <si>
+    <t>mcloseBrowser</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>waitFor</t>
+  </si>
+  <si>
+    <t>TS_010</t>
+  </si>
+  <si>
+    <t>TS_011</t>
+  </si>
+  <si>
+    <t>txt_Email</t>
+  </si>
+  <si>
+    <t>txt_Password</t>
+  </si>
+  <si>
+    <t>btn_Login</t>
+  </si>
+  <si>
+    <t>Click on login button</t>
+  </si>
+  <si>
+    <t>Chakradhar23342</t>
+  </si>
+  <si>
+    <t>Mobile Web Testing Facebook Account</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
     <t>mopenBrowser</t>
-  </si>
-  <si>
-    <t>mverifyElement</t>
-  </si>
-  <si>
-    <t>minput</t>
-  </si>
-  <si>
-    <t>Click button btn_Createaccount</t>
-  </si>
-  <si>
-    <t>mclick</t>
-  </si>
-  <si>
-    <t>Enter First Name in First Name field</t>
-  </si>
-  <si>
-    <t>Verify the webelement txt_Firstname</t>
-  </si>
-  <si>
-    <t>Verify the webelement txt_Lastname</t>
-  </si>
-  <si>
-    <t>Enter Last Name in txt_Lastname field</t>
-  </si>
-  <si>
-    <t>Ravikanth</t>
-  </si>
-  <si>
-    <t>Edamakanti</t>
-  </si>
-  <si>
-    <t>Click on Next button</t>
-  </si>
-  <si>
-    <t>Navigate to Facebook</t>
-  </si>
-  <si>
-    <t>mnavigate</t>
-  </si>
-  <si>
-    <t>Mobile_Facebook</t>
-  </si>
-  <si>
-    <t>Web Testing Facebook Account</t>
-  </si>
-  <si>
-    <t>Web_Facebook</t>
-  </si>
-  <si>
-    <t>Testing Facebook using Real Mobile Phone</t>
-  </si>
-  <si>
-    <t>Testing Facebook using Web Browser</t>
-  </si>
-  <si>
-    <t>TS_002</t>
-  </si>
-  <si>
-    <t>openBrowser</t>
-  </si>
-  <si>
-    <t>navigate</t>
-  </si>
-  <si>
-    <t>m_btn_Createaccount</t>
-  </si>
-  <si>
-    <t>m_txt_Firstname</t>
-  </si>
-  <si>
-    <t>m_txt_Lastname</t>
-  </si>
-  <si>
-    <t>m_btn_Next</t>
-  </si>
-  <si>
-    <t>verifyElement</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>click</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>Close Broswer</t>
-  </si>
-  <si>
-    <t>closeBrowser</t>
-  </si>
-  <si>
-    <t>TS_009</t>
-  </si>
-  <si>
-    <t>mcloseBrowser</t>
-  </si>
-  <si>
-    <t>Wait</t>
-  </si>
-  <si>
-    <t>waitFor</t>
-  </si>
-  <si>
-    <t>TS_010</t>
-  </si>
-  <si>
-    <t>TS_011</t>
-  </si>
-  <si>
-    <t>txt_Email</t>
-  </si>
-  <si>
-    <t>txt_Password</t>
-  </si>
-  <si>
-    <t>btn_Login</t>
-  </si>
-  <si>
-    <t>Click on login button</t>
-  </si>
-  <si>
-    <t>Chakradhar23342</t>
-  </si>
-  <si>
-    <t>Mobile Web Testing Facebook Account</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,7 +713,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -724,7 +724,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>2</v>
@@ -734,222 +734,222 @@
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="F3" s="11"/>
       <c r="G3" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>22</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -960,7 +960,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>2</v>
@@ -970,200 +970,200 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="11"/>
       <c r="E16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="E24" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1219,30 +1219,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>